<commit_message>
used new tagged and standardized colorado address files to test the tagger accuracy
</commit_message>
<xml_diff>
--- a/data/tagged colorado Stores.xlsx
+++ b/data/tagged colorado Stores.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3452" uniqueCount="1037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3456" uniqueCount="1041">
   <si>
     <t>17034 Highway 17</t>
   </si>
@@ -3133,6 +3133,18 @@
   </si>
   <si>
     <t>Record_ID</t>
+  </si>
+  <si>
+    <t>742 1/2</t>
+  </si>
+  <si>
+    <t>965 1/2</t>
+  </si>
+  <si>
+    <t>45 1/2</t>
+  </si>
+  <si>
+    <t>041290</t>
   </si>
 </sst>
 </file>
@@ -3186,7 +3198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3197,10 +3209,13 @@
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="12" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -3513,8 +3528,8 @@
   <dimension ref="A1:L507"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F236" sqref="F236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10220,8 +10235,8 @@
       <c r="E232" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F232" s="4">
-        <v>742.5</v>
+      <c r="F232" s="5" t="s">
+        <v>1037</v>
       </c>
       <c r="G232" s="3"/>
       <c r="H232" s="1" t="s">
@@ -10302,8 +10317,8 @@
       <c r="E235" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="F235" s="1">
-        <v>41290</v>
+      <c r="F235" s="6" t="s">
+        <v>1040</v>
       </c>
       <c r="H235" s="1">
         <v>6</v>
@@ -14895,7 +14910,7 @@
       <c r="K391" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="L391" s="5" t="s">
+      <c r="L391" s="4" t="s">
         <v>1028</v>
       </c>
     </row>
@@ -16127,8 +16142,8 @@
       <c r="E434" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F434" s="4">
-        <v>965.5</v>
+      <c r="F434" s="5" t="s">
+        <v>1038</v>
       </c>
       <c r="G434" s="3"/>
       <c r="H434" s="1" t="s">
@@ -17296,8 +17311,8 @@
       <c r="F475" s="1">
         <v>2185</v>
       </c>
-      <c r="H475" s="4">
-        <v>45.5</v>
+      <c r="H475" s="5" t="s">
+        <v>1039</v>
       </c>
       <c r="I475" s="1" t="s">
         <v>740</v>

</xml_diff>